<commit_message>
Versão submetida ao professor Marcelo em 21/12
</commit_message>
<xml_diff>
--- a/Cronograma.xlsx
+++ b/Cronograma.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\tex\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="18195" windowHeight="12075"/>
   </bookViews>
@@ -16,43 +21,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>Coleta de evidências</t>
+    <t>Jan/18</t>
   </si>
   <si>
-    <t>Proposição do método</t>
+    <t>Fev/18</t>
   </si>
   <si>
-    <t>Implementação-modelo do método proposto</t>
+    <t>Mar/18</t>
   </si>
   <si>
-    <t>Avaliação do método</t>
+    <t>Mapeamento de cenários</t>
   </si>
   <si>
-    <t>Síntese dos resultados</t>
+    <t>Especificação da proposta</t>
   </si>
   <si>
-    <t>Abril/17</t>
+    <t>Implementação</t>
   </si>
   <si>
-    <t>Maio/17</t>
+    <t>Validação</t>
   </si>
   <si>
-    <t>Junho/17</t>
-  </si>
-  <si>
-    <t>Julho/17</t>
-  </si>
-  <si>
-    <t>Agosto/17</t>
+    <t>Abr/18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,6 +61,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -87,20 +92,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -112,6 +121,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -120,14 +132,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>790575</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
@@ -138,7 +150,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2752725" y="247650"/>
+          <a:off x="1695450" y="247650"/>
           <a:ext cx="752475" cy="238125"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -175,14 +187,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>200024</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>476251</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>171449</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>790575</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>314325</xdr:rowOff>
     </xdr:to>
@@ -193,8 +205,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495674" y="647700"/>
-          <a:ext cx="790575" cy="238125"/>
+          <a:off x="2524126" y="647700"/>
+          <a:ext cx="1133474" cy="238125"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -230,14 +242,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>809624</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>790575</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>314325</xdr:rowOff>
     </xdr:to>
@@ -248,8 +260,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3838575" y="1038225"/>
-          <a:ext cx="1085849" cy="238125"/>
+          <a:off x="3171825" y="1038225"/>
+          <a:ext cx="1304925" cy="238125"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -286,13 +298,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>428623</xdr:colOff>
+      <xdr:colOff>28574</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>352424</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>428626</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
@@ -303,63 +315,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4543423" y="1419225"/>
-          <a:ext cx="742951" cy="238125"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="6350"/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="pt-BR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>809624</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>314325</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Retângulo 5"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5295900" y="1819275"/>
-          <a:ext cx="447674" cy="238125"/>
+          <a:off x="4533899" y="1419225"/>
+          <a:ext cx="400052" cy="238125"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -399,7 +356,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -437,9 +394,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -474,7 +431,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -509,7 +466,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -683,89 +640,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" style="1" customWidth="1"/>
-    <col min="2" max="6" width="12.28515625" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="30.7109375" style="1" customWidth="1"/>
+    <col min="2" max="5" width="12.28515625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="4294967294" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>